<commit_message>
[jms] - move websphere-specific code to java reflection-based code to remove dependencies
Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/artifact/script/rdbms-01.xlsx
+++ b/artifact/script/rdbms-01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="500" windowHeight="12540" windowWidth="40960" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="12980"/>
+    <workbookView activeTab="1" tabRatio="500" windowHeight="12540" windowWidth="40960" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="12980" firstSheet="1"/>
   </bookViews>
   <sheets>
     <sheet name="#system" r:id="rId1" sheetId="4" state="hidden"/>
@@ -36,12 +36,13 @@
     <definedName name="pdf">'#system'!$N$2:$N$16</definedName>
     <definedName name="rdbms">'#system'!$O$2:$O$6</definedName>
     <definedName name="ssh">'#system'!$P$2:$P$9</definedName>
-    <definedName name="target">'#system'!$A$2:$A$21</definedName>
-    <definedName name="web">'#system'!$Q$2:$Q$108</definedName>
-    <definedName name="webalert">'#system'!$R$2:$R$6</definedName>
-    <definedName name="webcookie">'#system'!$S$2:$S$8</definedName>
-    <definedName name="ws">'#system'!$T$2:$T$16</definedName>
-    <definedName name="xml">'#system'!$U$2:$U$11</definedName>
+    <definedName name="target">'#system'!$A$2:$A$22</definedName>
+    <definedName name="web">'#system'!$R$2:$R$108</definedName>
+    <definedName name="webalert">'#system'!$S$2:$S$6</definedName>
+    <definedName name="webcookie">'#system'!$T$2:$T$8</definedName>
+    <definedName name="ws">'#system'!$U$2:$U$16</definedName>
+    <definedName name="xml">'#system'!$V$2:$V$11</definedName>
+    <definedName name="step">'#system'!$Q$2:$Q$4</definedName>
   </definedNames>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2048" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2462" uniqueCount="415">
   <si>
     <t>jira</t>
   </si>
@@ -1283,6 +1284,24 @@
   </si>
   <si>
     <t>assertBetween(num,lower,upper)</t>
+  </si>
+  <si>
+    <t>story / feature</t>
+  </si>
+  <si>
+    <t>test id</t>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>observe(prompt)</t>
+  </si>
+  <si>
+    <t>perform(instructions)</t>
+  </si>
+  <si>
+    <t>validate(prompt,responses,passResponses)</t>
   </si>
 </sst>
 </file>
@@ -1290,7 +1309,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="59" x14ac:knownFonts="1">
+  <fonts count="71" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1671,8 +1690,84 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="88">
+  <fills count="109">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2167,8 +2262,127 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="83">
+  <borders count="103">
     <border>
       <left/>
       <right/>
@@ -2982,6 +3196,200 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -2989,7 +3397,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="97">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -3226,40 +3634,76 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="46" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="69" borderId="70" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="70" fillId="69" fontId="47" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="48" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="72" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="72" fontId="49" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="50" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="75" borderId="74" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="74" fillId="75" fontId="51" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="78" borderId="78" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="78" fillId="78" fontId="52" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="81" borderId="82" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="82" fillId="81" fontId="53" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="81" borderId="82" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="82" fillId="81" fontId="54" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="84" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="84" fontId="55" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="87" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="87" fontId="56" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="84" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="84" fontId="57" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="58" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="90" borderId="90" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="93" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="96" borderId="94" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="99" borderId="98" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="102" borderId="102" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="102" borderId="102" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="105" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="108" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="105" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3584,9 +4028,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V108"/>
+  <dimension ref="A1:W108"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
+    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" tabSelected="false">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -3645,18 +4089,21 @@
         <v>363</v>
       </c>
       <c r="Q1" t="s">
+        <v>411</v>
+      </c>
+      <c r="R1" t="s">
         <v>56</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>57</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>58</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>59</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>231</v>
       </c>
     </row>
@@ -3710,18 +4157,21 @@
         <v>387</v>
       </c>
       <c r="Q2" t="s">
+        <v>412</v>
+      </c>
+      <c r="R2" t="s">
         <v>99</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>174</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>179</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>186</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>232</v>
       </c>
     </row>
@@ -3772,18 +4222,21 @@
         <v>388</v>
       </c>
       <c r="Q3" t="s">
+        <v>413</v>
+      </c>
+      <c r="R3" t="s">
         <v>100</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>175</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>180</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>370</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>233</v>
       </c>
     </row>
@@ -3831,18 +4284,21 @@
         <v>364</v>
       </c>
       <c r="Q4" t="s">
+        <v>414</v>
+      </c>
+      <c r="R4" t="s">
         <v>358</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>176</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>181</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>187</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>234</v>
       </c>
     </row>
@@ -3883,19 +4339,19 @@
       <c r="P5" t="s">
         <v>365</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>359</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>177</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>182</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>188</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>235</v>
       </c>
     </row>
@@ -3933,19 +4389,19 @@
       <c r="P6" t="s">
         <v>367</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>101</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>178</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>183</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>189</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>236</v>
       </c>
     </row>
@@ -3980,16 +4436,16 @@
       <c r="P7" t="s">
         <v>366</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>102</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>184</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>190</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>237</v>
       </c>
     </row>
@@ -4024,16 +4480,16 @@
       <c r="P8" t="s">
         <v>368</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>103</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>185</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>191</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>238</v>
       </c>
     </row>
@@ -4065,13 +4521,13 @@
       <c r="P9" t="s">
         <v>369</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>213</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>192</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>239</v>
       </c>
     </row>
@@ -4097,13 +4553,13 @@
       <c r="N10" t="s">
         <v>251</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>261</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>193</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>240</v>
       </c>
     </row>
@@ -4129,13 +4585,13 @@
       <c r="N11" t="s">
         <v>252</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>262</v>
       </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
         <v>263</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>241</v>
       </c>
     </row>
@@ -4158,10 +4614,10 @@
       <c r="N12" t="s">
         <v>253</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>104</v>
       </c>
-      <c r="T12" t="s">
+      <c r="U12" t="s">
         <v>194</v>
       </c>
     </row>
@@ -4184,10 +4640,10 @@
       <c r="N13" t="s">
         <v>258</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>330</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4210,10 +4666,10 @@
       <c r="N14" t="s">
         <v>254</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>105</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>196</v>
       </c>
     </row>
@@ -4233,10 +4689,10 @@
       <c r="N15" t="s">
         <v>255</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>106</v>
       </c>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
         <v>197</v>
       </c>
     </row>
@@ -4256,16 +4712,16 @@
       <c r="N16" t="s">
         <v>256</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>77</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>411</v>
       </c>
       <c r="C17" t="s">
         <v>63</v>
@@ -4276,13 +4732,13 @@
       <c r="I17" t="s">
         <v>46</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
         <v>260</v>
@@ -4293,13 +4749,13 @@
       <c r="I18" t="s">
         <v>405</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="R18" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
         <v>64</v>
@@ -4310,13 +4766,13 @@
       <c r="I19" t="s">
         <v>87</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="R19" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
         <v>325</v>
@@ -4327,13 +4783,13 @@
       <c r="I20" t="s">
         <v>47</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>231</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
         <v>65</v>
@@ -4344,18 +4800,21 @@
       <c r="I21" t="s">
         <v>48</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="R21" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="22">
+      <c r="A22" t="s">
+        <v>231</v>
+      </c>
       <c r="C22" t="s">
         <v>229</v>
       </c>
       <c r="E22" t="s">
         <v>303</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="R22" t="s">
         <v>112</v>
       </c>
     </row>
@@ -4366,7 +4825,7 @@
       <c r="E23" t="s">
         <v>294</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="R23" t="s">
         <v>113</v>
       </c>
     </row>
@@ -4377,7 +4836,7 @@
       <c r="E24" t="s">
         <v>283</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="R24" t="s">
         <v>114</v>
       </c>
     </row>
@@ -4388,7 +4847,7 @@
       <c r="E25" t="s">
         <v>78</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="R25" t="s">
         <v>115</v>
       </c>
     </row>
@@ -4399,7 +4858,7 @@
       <c r="E26" t="s">
         <v>286</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="R26" t="s">
         <v>116</v>
       </c>
     </row>
@@ -4410,7 +4869,7 @@
       <c r="E27" t="s">
         <v>270</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="R27" t="s">
         <v>331</v>
       </c>
     </row>
@@ -4421,7 +4880,7 @@
       <c r="E28" t="s">
         <v>287</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="R28" t="s">
         <v>117</v>
       </c>
     </row>
@@ -4432,7 +4891,7 @@
       <c r="E29" t="s">
         <v>288</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="R29" t="s">
         <v>118</v>
       </c>
     </row>
@@ -4443,7 +4902,7 @@
       <c r="E30" t="s">
         <v>220</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="R30" t="s">
         <v>119</v>
       </c>
     </row>
@@ -4454,7 +4913,7 @@
       <c r="E31" t="s">
         <v>279</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="R31" t="s">
         <v>120</v>
       </c>
     </row>
@@ -4462,7 +4921,7 @@
       <c r="E32" t="s">
         <v>289</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="R32" t="s">
         <v>121</v>
       </c>
     </row>
@@ -4470,7 +4929,7 @@
       <c r="E33" t="s">
         <v>264</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="R33" t="s">
         <v>122</v>
       </c>
     </row>
@@ -4478,7 +4937,7 @@
       <c r="E34" t="s">
         <v>334</v>
       </c>
-      <c r="Q34" t="s">
+      <c r="R34" t="s">
         <v>214</v>
       </c>
     </row>
@@ -4486,7 +4945,7 @@
       <c r="E35" t="s">
         <v>311</v>
       </c>
-      <c r="Q35" t="s">
+      <c r="R35" t="s">
         <v>123</v>
       </c>
     </row>
@@ -4494,7 +4953,7 @@
       <c r="E36" t="s">
         <v>265</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="R36" t="s">
         <v>342</v>
       </c>
     </row>
@@ -4502,7 +4961,7 @@
       <c r="E37" t="s">
         <v>312</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="R37" t="s">
         <v>406</v>
       </c>
     </row>
@@ -4510,7 +4969,7 @@
       <c r="E38" t="s">
         <v>271</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="R38" t="s">
         <v>124</v>
       </c>
     </row>
@@ -4518,7 +4977,7 @@
       <c r="E39" t="s">
         <v>80</v>
       </c>
-      <c r="Q39" t="s">
+      <c r="R39" t="s">
         <v>125</v>
       </c>
     </row>
@@ -4526,7 +4985,7 @@
       <c r="E40" t="s">
         <v>216</v>
       </c>
-      <c r="Q40" t="s">
+      <c r="R40" t="s">
         <v>126</v>
       </c>
     </row>
@@ -4534,7 +4993,7 @@
       <c r="E41" t="s">
         <v>293</v>
       </c>
-      <c r="Q41" t="s">
+      <c r="R41" t="s">
         <v>127</v>
       </c>
     </row>
@@ -4542,7 +5001,7 @@
       <c r="E42" t="s">
         <v>304</v>
       </c>
-      <c r="Q42" t="s">
+      <c r="R42" t="s">
         <v>128</v>
       </c>
     </row>
@@ -4550,7 +5009,7 @@
       <c r="E43" t="s">
         <v>305</v>
       </c>
-      <c r="Q43" t="s">
+      <c r="R43" t="s">
         <v>129</v>
       </c>
     </row>
@@ -4558,7 +5017,7 @@
       <c r="E44" t="s">
         <v>347</v>
       </c>
-      <c r="Q44" t="s">
+      <c r="R44" t="s">
         <v>217</v>
       </c>
     </row>
@@ -4566,7 +5025,7 @@
       <c r="E45" t="s">
         <v>346</v>
       </c>
-      <c r="Q45" t="s">
+      <c r="R45" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4574,7 +5033,7 @@
       <c r="E46" t="s">
         <v>215</v>
       </c>
-      <c r="Q46" t="s">
+      <c r="R46" t="s">
         <v>130</v>
       </c>
     </row>
@@ -4582,7 +5041,7 @@
       <c r="E47" t="s">
         <v>324</v>
       </c>
-      <c r="Q47" t="s">
+      <c r="R47" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4590,7 +5049,7 @@
       <c r="E48" t="s">
         <v>343</v>
       </c>
-      <c r="Q48" t="s">
+      <c r="R48" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4598,7 +5057,7 @@
       <c r="E49" t="s">
         <v>374</v>
       </c>
-      <c r="Q49" t="s">
+      <c r="R49" t="s">
         <v>133</v>
       </c>
     </row>
@@ -4606,7 +5065,7 @@
       <c r="E50" t="s">
         <v>306</v>
       </c>
-      <c r="Q50" t="s">
+      <c r="R50" t="s">
         <v>350</v>
       </c>
     </row>
@@ -4614,7 +5073,7 @@
       <c r="E51" t="s">
         <v>360</v>
       </c>
-      <c r="Q51" t="s">
+      <c r="R51" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4622,7 +5081,7 @@
       <c r="E52" t="s">
         <v>361</v>
       </c>
-      <c r="Q52" t="s">
+      <c r="R52" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4630,7 +5089,7 @@
       <c r="E53" t="s">
         <v>362</v>
       </c>
-      <c r="Q53" t="s">
+      <c r="R53" t="s">
         <v>136</v>
       </c>
     </row>
@@ -4638,7 +5097,7 @@
       <c r="E54" t="s">
         <v>335</v>
       </c>
-      <c r="Q54" t="s">
+      <c r="R54" t="s">
         <v>137</v>
       </c>
     </row>
@@ -4646,7 +5105,7 @@
       <c r="E55" t="s">
         <v>272</v>
       </c>
-      <c r="Q55" t="s">
+      <c r="R55" t="s">
         <v>138</v>
       </c>
     </row>
@@ -4654,7 +5113,7 @@
       <c r="E56" t="s">
         <v>296</v>
       </c>
-      <c r="Q56" t="s">
+      <c r="R56" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4662,7 +5121,7 @@
       <c r="E57" t="s">
         <v>297</v>
       </c>
-      <c r="Q57" t="s">
+      <c r="R57" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4670,7 +5129,7 @@
       <c r="E58" t="s">
         <v>298</v>
       </c>
-      <c r="Q58" t="s">
+      <c r="R58" t="s">
         <v>218</v>
       </c>
     </row>
@@ -4678,7 +5137,7 @@
       <c r="E59" t="s">
         <v>307</v>
       </c>
-      <c r="Q59" t="s">
+      <c r="R59" t="s">
         <v>395</v>
       </c>
     </row>
@@ -4686,7 +5145,7 @@
       <c r="E60" t="s">
         <v>316</v>
       </c>
-      <c r="Q60" t="s">
+      <c r="R60" t="s">
         <v>141</v>
       </c>
     </row>
@@ -4694,7 +5153,7 @@
       <c r="E61" t="s">
         <v>341</v>
       </c>
-      <c r="Q61" t="s">
+      <c r="R61" t="s">
         <v>142</v>
       </c>
     </row>
@@ -4702,7 +5161,7 @@
       <c r="E62" t="s">
         <v>313</v>
       </c>
-      <c r="Q62" t="s">
+      <c r="R62" t="s">
         <v>143</v>
       </c>
     </row>
@@ -4710,7 +5169,7 @@
       <c r="E63" t="s">
         <v>314</v>
       </c>
-      <c r="Q63" t="s">
+      <c r="R63" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4718,7 +5177,7 @@
       <c r="E64" t="s">
         <v>375</v>
       </c>
-      <c r="Q64" t="s">
+      <c r="R64" t="s">
         <v>201</v>
       </c>
     </row>
@@ -4726,7 +5185,7 @@
       <c r="E65" t="s">
         <v>376</v>
       </c>
-      <c r="Q65" t="s">
+      <c r="R65" t="s">
         <v>202</v>
       </c>
     </row>
@@ -4734,7 +5193,7 @@
       <c r="E66" t="s">
         <v>349</v>
       </c>
-      <c r="Q66" t="s">
+      <c r="R66" t="s">
         <v>145</v>
       </c>
     </row>
@@ -4742,7 +5201,7 @@
       <c r="E67" t="s">
         <v>317</v>
       </c>
-      <c r="Q67" t="s">
+      <c r="R67" t="s">
         <v>146</v>
       </c>
     </row>
@@ -4750,7 +5209,7 @@
       <c r="E68" t="s">
         <v>273</v>
       </c>
-      <c r="Q68" t="s">
+      <c r="R68" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4758,7 +5217,7 @@
       <c r="E69" t="s">
         <v>357</v>
       </c>
-      <c r="Q69" t="s">
+      <c r="R69" t="s">
         <v>148</v>
       </c>
     </row>
@@ -4766,7 +5225,7 @@
       <c r="E70" t="s">
         <v>318</v>
       </c>
-      <c r="Q70" t="s">
+      <c r="R70" t="s">
         <v>149</v>
       </c>
     </row>
@@ -4774,7 +5233,7 @@
       <c r="E71" t="s">
         <v>308</v>
       </c>
-      <c r="Q71" t="s">
+      <c r="R71" t="s">
         <v>203</v>
       </c>
     </row>
@@ -4782,7 +5241,7 @@
       <c r="E72" t="s">
         <v>266</v>
       </c>
-      <c r="Q72" t="s">
+      <c r="R72" t="s">
         <v>204</v>
       </c>
     </row>
@@ -4790,7 +5249,7 @@
       <c r="E73" t="s">
         <v>348</v>
       </c>
-      <c r="Q73" t="s">
+      <c r="R73" t="s">
         <v>205</v>
       </c>
     </row>
@@ -4798,7 +5257,7 @@
       <c r="E74" t="s">
         <v>284</v>
       </c>
-      <c r="Q74" t="s">
+      <c r="R74" t="s">
         <v>206</v>
       </c>
     </row>
@@ -4806,7 +5265,7 @@
       <c r="E75" t="s">
         <v>290</v>
       </c>
-      <c r="Q75" t="s">
+      <c r="R75" t="s">
         <v>219</v>
       </c>
     </row>
@@ -4814,7 +5273,7 @@
       <c r="E76" t="s">
         <v>295</v>
       </c>
-      <c r="Q76" t="s">
+      <c r="R76" t="s">
         <v>150</v>
       </c>
     </row>
@@ -4822,7 +5281,7 @@
       <c r="E77" t="s">
         <v>336</v>
       </c>
-      <c r="Q77" t="s">
+      <c r="R77" t="s">
         <v>207</v>
       </c>
     </row>
@@ -4830,7 +5289,7 @@
       <c r="E78" t="s">
         <v>274</v>
       </c>
-      <c r="Q78" t="s">
+      <c r="R78" t="s">
         <v>151</v>
       </c>
     </row>
@@ -4838,7 +5297,7 @@
       <c r="E79" t="s">
         <v>285</v>
       </c>
-      <c r="Q79" t="s">
+      <c r="R79" t="s">
         <v>208</v>
       </c>
     </row>
@@ -4846,7 +5305,7 @@
       <c r="E80" t="s">
         <v>291</v>
       </c>
-      <c r="Q80" t="s">
+      <c r="R80" t="s">
         <v>209</v>
       </c>
     </row>
@@ -4854,7 +5313,7 @@
       <c r="E81" t="s">
         <v>280</v>
       </c>
-      <c r="Q81" t="s">
+      <c r="R81" t="s">
         <v>210</v>
       </c>
     </row>
@@ -4862,7 +5321,7 @@
       <c r="E82" t="s">
         <v>275</v>
       </c>
-      <c r="Q82" t="s">
+      <c r="R82" t="s">
         <v>211</v>
       </c>
     </row>
@@ -4870,7 +5329,7 @@
       <c r="E83" t="s">
         <v>292</v>
       </c>
-      <c r="Q83" t="s">
+      <c r="R83" t="s">
         <v>227</v>
       </c>
     </row>
@@ -4878,7 +5337,7 @@
       <c r="E84" t="s">
         <v>276</v>
       </c>
-      <c r="Q84" t="s">
+      <c r="R84" t="s">
         <v>212</v>
       </c>
     </row>
@@ -4886,7 +5345,7 @@
       <c r="E85" t="s">
         <v>277</v>
       </c>
-      <c r="Q85" t="s">
+      <c r="R85" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4894,7 +5353,7 @@
       <c r="E86" t="s">
         <v>309</v>
       </c>
-      <c r="Q86" t="s">
+      <c r="R86" t="s">
         <v>389</v>
       </c>
     </row>
@@ -4902,7 +5361,7 @@
       <c r="E87" t="s">
         <v>315</v>
       </c>
-      <c r="Q87" t="s">
+      <c r="R87" t="s">
         <v>153</v>
       </c>
     </row>
@@ -4910,7 +5369,7 @@
       <c r="E88" t="s">
         <v>299</v>
       </c>
-      <c r="Q88" t="s">
+      <c r="R88" t="s">
         <v>154</v>
       </c>
     </row>
@@ -4918,7 +5377,7 @@
       <c r="E89" t="s">
         <v>344</v>
       </c>
-      <c r="Q89" t="s">
+      <c r="R89" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4926,7 +5385,7 @@
       <c r="E90" t="s">
         <v>281</v>
       </c>
-      <c r="Q90" t="s">
+      <c r="R90" t="s">
         <v>156</v>
       </c>
     </row>
@@ -4934,92 +5393,92 @@
       <c r="E91" t="s">
         <v>282</v>
       </c>
-      <c r="Q91" t="s">
+      <c r="R91" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="92">
-      <c r="Q92" t="s">
+      <c r="R92" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="93">
-      <c r="Q93" t="s">
+      <c r="R93" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="94">
-      <c r="Q94" t="s">
+      <c r="R94" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="95">
-      <c r="Q95" t="s">
+      <c r="R95" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="96">
-      <c r="Q96" t="s">
+      <c r="R96" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="97">
-      <c r="Q97" t="s">
+      <c r="R97" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="98">
-      <c r="Q98" t="s">
+      <c r="R98" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="99">
-      <c r="Q99" t="s">
+      <c r="R99" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="100">
-      <c r="Q100" t="s">
+      <c r="R100" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="101">
-      <c r="Q101" t="s">
+      <c r="R101" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="102">
-      <c r="Q102" t="s">
+      <c r="R102" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="103">
-      <c r="Q103" t="s">
+      <c r="R103" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="104">
-      <c r="Q104" t="s">
+      <c r="R104" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="105">
-      <c r="Q105" t="s">
+      <c r="R105" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="106">
-      <c r="Q106" t="s">
+      <c r="R106" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="107">
-      <c r="Q107" t="s">
+      <c r="R107" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="108">
-      <c r="Q108" t="s">
+      <c r="R108" t="s">
         <v>173</v>
       </c>
     </row>
@@ -5032,9 +5491,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0" zoomScale="100">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A5" ySplit="4"/>
-      <selection activeCell="A2" pane="bottomLeft" sqref="A2:D2"/>
+      <selection activeCell="A5" pane="bottomLeft" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5067,10 +5526,10 @@
         <v>22</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>0</v>
+        <v>409</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>1</v>
+        <v>410</v>
       </c>
       <c r="I1" s="24" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
update test artifacts to nexial compatible
Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/artifact/script/rdbms-01.xlsx
+++ b/artifact/script/rdbms-01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="500" windowHeight="12540" windowWidth="40960" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="12980" firstSheet="1"/>
+    <workbookView activeTab="1" firstSheet="1" tabRatio="500" windowHeight="12540" windowWidth="40960" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="12980"/>
   </bookViews>
   <sheets>
     <sheet name="#system" r:id="rId1" sheetId="4" state="hidden"/>
@@ -21,7 +21,7 @@
     <definedName name="csv">'#system'!$D$2:$D$4</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$E$2:$E$91</definedName>
+    <definedName name="desktop">'#system'!$E$2:$E$90</definedName>
     <definedName name="excel">'#system'!$F$2:$F$8</definedName>
     <definedName name="external">'#system'!$G$2:$G$3</definedName>
     <definedName name="image">'#system'!$H$2:$H$5</definedName>
@@ -35,14 +35,15 @@
     <definedName name="number">'#system'!$M$2:$M$14</definedName>
     <definedName name="pdf">'#system'!$N$2:$N$16</definedName>
     <definedName name="rdbms">'#system'!$O$2:$O$6</definedName>
-    <definedName name="ssh">'#system'!$P$2:$P$9</definedName>
-    <definedName name="target">'#system'!$A$2:$A$22</definedName>
-    <definedName name="web">'#system'!$R$2:$R$108</definedName>
-    <definedName name="webalert">'#system'!$S$2:$S$6</definedName>
-    <definedName name="webcookie">'#system'!$T$2:$T$8</definedName>
-    <definedName name="ws">'#system'!$U$2:$U$16</definedName>
-    <definedName name="xml">'#system'!$V$2:$V$11</definedName>
-    <definedName name="step">'#system'!$Q$2:$Q$4</definedName>
+    <definedName name="ssh">'#system'!$Q$2:$Q$9</definedName>
+    <definedName name="target">'#system'!$A$2:$A$23</definedName>
+    <definedName name="web">'#system'!$S$2:$S$108</definedName>
+    <definedName name="webalert">'#system'!$T$2:$T$6</definedName>
+    <definedName name="webcookie">'#system'!$U$2:$U$8</definedName>
+    <definedName name="ws">'#system'!$V$2:$V$16</definedName>
+    <definedName name="xml">'#system'!$W$2:$W$11</definedName>
+    <definedName name="step">'#system'!$R$2:$R$4</definedName>
+    <definedName name="redis">'#system'!$P$2:$P$10</definedName>
   </definedNames>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2462" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2881" uniqueCount="426">
   <si>
     <t>jira</t>
   </si>
@@ -1302,6 +1303,39 @@
   </si>
   <si>
     <t>validate(prompt,responses,passResponses)</t>
+  </si>
+  <si>
+    <t>redis</t>
+  </si>
+  <si>
+    <t>saveTableRowsRange(var,beginRow,endRow)</t>
+  </si>
+  <si>
+    <t>append(profile,key,value)</t>
+  </si>
+  <si>
+    <t>assertKeyExists(profile,key)</t>
+  </si>
+  <si>
+    <t>delete(profile,key)</t>
+  </si>
+  <si>
+    <t>flushAll(profile)</t>
+  </si>
+  <si>
+    <t>flushDb(profile)</t>
+  </si>
+  <si>
+    <t>rename(profile,current,new)</t>
+  </si>
+  <si>
+    <t>set(profile,key,value)</t>
+  </si>
+  <si>
+    <t>store(var,profile,key)</t>
+  </si>
+  <si>
+    <t>storeKeys(var,profile,keyPattern)</t>
   </si>
 </sst>
 </file>
@@ -1309,7 +1343,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="71" x14ac:knownFonts="1">
+  <fonts count="83" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1766,8 +1800,84 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="109">
+  <fills count="130">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2381,8 +2491,127 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="103">
+  <borders count="123">
     <border>
       <left/>
       <right/>
@@ -3390,6 +3619,200 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -3397,7 +3820,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="109">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -3670,40 +4093,76 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="58" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="90" borderId="90" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="90" fillId="90" fontId="59" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="60" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="93" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="93" fontId="61" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="62" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="63" fillId="96" borderId="94" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="94" fillId="96" fontId="63" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="64" fillId="99" borderId="98" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="98" fillId="99" fontId="64" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="102" borderId="102" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="102" fillId="102" fontId="65" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="66" fillId="102" borderId="102" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="102" fillId="102" fontId="66" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="105" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="105" fontId="67" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="108" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="108" fontId="68" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="105" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="105" fontId="69" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="70" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="111" borderId="110" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="114" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="117" borderId="114" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="120" borderId="118" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="123" borderId="122" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="123" borderId="122" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="79" fillId="126" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="129" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="126" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4028,9 +4487,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W108"/>
+  <dimension ref="A1:X108"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" tabSelected="false">
+    <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -4086,24 +4545,27 @@
         <v>55</v>
       </c>
       <c r="P1" t="s">
+        <v>415</v>
+      </c>
+      <c r="Q1" t="s">
         <v>363</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>411</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>56</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>57</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>58</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>59</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>231</v>
       </c>
     </row>
@@ -4154,24 +4616,27 @@
         <v>221</v>
       </c>
       <c r="P2" t="s">
+        <v>417</v>
+      </c>
+      <c r="Q2" t="s">
         <v>387</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>412</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>99</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>174</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>179</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>186</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>232</v>
       </c>
     </row>
@@ -4219,24 +4684,27 @@
         <v>222</v>
       </c>
       <c r="P3" t="s">
+        <v>418</v>
+      </c>
+      <c r="Q3" t="s">
         <v>388</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>413</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>100</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>175</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>180</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>370</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>233</v>
       </c>
     </row>
@@ -4281,24 +4749,27 @@
         <v>223</v>
       </c>
       <c r="P4" t="s">
+        <v>419</v>
+      </c>
+      <c r="Q4" t="s">
         <v>364</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>414</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>358</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>176</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>181</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>187</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>234</v>
       </c>
     </row>
@@ -4337,21 +4808,24 @@
         <v>224</v>
       </c>
       <c r="P5" t="s">
+        <v>420</v>
+      </c>
+      <c r="Q5" t="s">
         <v>365</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>359</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>177</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>182</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>188</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>235</v>
       </c>
     </row>
@@ -4387,21 +4861,24 @@
         <v>397</v>
       </c>
       <c r="P6" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q6" t="s">
         <v>367</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>101</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>178</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>183</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>189</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>236</v>
       </c>
     </row>
@@ -4434,18 +4911,21 @@
         <v>248</v>
       </c>
       <c r="P7" t="s">
+        <v>422</v>
+      </c>
+      <c r="Q7" t="s">
         <v>366</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>102</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>184</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>190</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>237</v>
       </c>
     </row>
@@ -4478,18 +4958,21 @@
         <v>249</v>
       </c>
       <c r="P8" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q8" t="s">
         <v>368</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>103</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>185</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>191</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>238</v>
       </c>
     </row>
@@ -4519,15 +5002,18 @@
         <v>250</v>
       </c>
       <c r="P9" t="s">
+        <v>424</v>
+      </c>
+      <c r="Q9" t="s">
         <v>369</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>213</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>192</v>
       </c>
-      <c r="V9" t="s">
+      <c r="W9" t="s">
         <v>239</v>
       </c>
     </row>
@@ -4553,13 +5039,16 @@
       <c r="N10" t="s">
         <v>251</v>
       </c>
-      <c r="R10" t="s">
+      <c r="P10" t="s">
+        <v>425</v>
+      </c>
+      <c r="S10" t="s">
         <v>261</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>193</v>
       </c>
-      <c r="V10" t="s">
+      <c r="W10" t="s">
         <v>240</v>
       </c>
     </row>
@@ -4585,13 +5074,13 @@
       <c r="N11" t="s">
         <v>252</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>262</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>263</v>
       </c>
-      <c r="V11" t="s">
+      <c r="W11" t="s">
         <v>241</v>
       </c>
     </row>
@@ -4614,10 +5103,10 @@
       <c r="N12" t="s">
         <v>253</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>104</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>194</v>
       </c>
     </row>
@@ -4640,10 +5129,10 @@
       <c r="N13" t="s">
         <v>258</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>330</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4666,10 +5155,10 @@
       <c r="N14" t="s">
         <v>254</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>105</v>
       </c>
-      <c r="U14" t="s">
+      <c r="V14" t="s">
         <v>196</v>
       </c>
     </row>
@@ -4689,16 +5178,16 @@
       <c r="N15" t="s">
         <v>255</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>106</v>
       </c>
-      <c r="U15" t="s">
+      <c r="V15" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>363</v>
+        <v>415</v>
       </c>
       <c r="C16" t="s">
         <v>62</v>
@@ -4712,16 +5201,16 @@
       <c r="N16" t="s">
         <v>256</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>77</v>
       </c>
-      <c r="U16" t="s">
+      <c r="V16" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>411</v>
+        <v>363</v>
       </c>
       <c r="C17" t="s">
         <v>63</v>
@@ -4732,13 +5221,13 @@
       <c r="I17" t="s">
         <v>46</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>411</v>
       </c>
       <c r="C18" t="s">
         <v>260</v>
@@ -4749,13 +5238,13 @@
       <c r="I18" t="s">
         <v>405</v>
       </c>
-      <c r="R18" t="s">
+      <c r="S18" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
         <v>64</v>
@@ -4766,13 +5255,13 @@
       <c r="I19" t="s">
         <v>87</v>
       </c>
-      <c r="R19" t="s">
+      <c r="S19" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
         <v>325</v>
@@ -4783,13 +5272,13 @@
       <c r="I20" t="s">
         <v>47</v>
       </c>
-      <c r="R20" t="s">
+      <c r="S20" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
         <v>65</v>
@@ -4800,13 +5289,13 @@
       <c r="I21" t="s">
         <v>48</v>
       </c>
-      <c r="R21" t="s">
+      <c r="S21" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>231</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
         <v>229</v>
@@ -4814,18 +5303,21 @@
       <c r="E22" t="s">
         <v>303</v>
       </c>
-      <c r="R22" t="s">
+      <c r="S22" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="23">
+      <c r="A23" t="s">
+        <v>231</v>
+      </c>
       <c r="C23" t="s">
         <v>230</v>
       </c>
       <c r="E23" t="s">
         <v>294</v>
       </c>
-      <c r="R23" t="s">
+      <c r="S23" t="s">
         <v>113</v>
       </c>
     </row>
@@ -4836,7 +5328,7 @@
       <c r="E24" t="s">
         <v>283</v>
       </c>
-      <c r="R24" t="s">
+      <c r="S24" t="s">
         <v>114</v>
       </c>
     </row>
@@ -4847,7 +5339,7 @@
       <c r="E25" t="s">
         <v>78</v>
       </c>
-      <c r="R25" t="s">
+      <c r="S25" t="s">
         <v>115</v>
       </c>
     </row>
@@ -4858,7 +5350,7 @@
       <c r="E26" t="s">
         <v>286</v>
       </c>
-      <c r="R26" t="s">
+      <c r="S26" t="s">
         <v>116</v>
       </c>
     </row>
@@ -4869,7 +5361,7 @@
       <c r="E27" t="s">
         <v>270</v>
       </c>
-      <c r="R27" t="s">
+      <c r="S27" t="s">
         <v>331</v>
       </c>
     </row>
@@ -4880,7 +5372,7 @@
       <c r="E28" t="s">
         <v>287</v>
       </c>
-      <c r="R28" t="s">
+      <c r="S28" t="s">
         <v>117</v>
       </c>
     </row>
@@ -4891,7 +5383,7 @@
       <c r="E29" t="s">
         <v>288</v>
       </c>
-      <c r="R29" t="s">
+      <c r="S29" t="s">
         <v>118</v>
       </c>
     </row>
@@ -4902,7 +5394,7 @@
       <c r="E30" t="s">
         <v>220</v>
       </c>
-      <c r="R30" t="s">
+      <c r="S30" t="s">
         <v>119</v>
       </c>
     </row>
@@ -4913,7 +5405,7 @@
       <c r="E31" t="s">
         <v>279</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S31" t="s">
         <v>120</v>
       </c>
     </row>
@@ -4921,7 +5413,7 @@
       <c r="E32" t="s">
         <v>289</v>
       </c>
-      <c r="R32" t="s">
+      <c r="S32" t="s">
         <v>121</v>
       </c>
     </row>
@@ -4929,7 +5421,7 @@
       <c r="E33" t="s">
         <v>264</v>
       </c>
-      <c r="R33" t="s">
+      <c r="S33" t="s">
         <v>122</v>
       </c>
     </row>
@@ -4937,7 +5429,7 @@
       <c r="E34" t="s">
         <v>334</v>
       </c>
-      <c r="R34" t="s">
+      <c r="S34" t="s">
         <v>214</v>
       </c>
     </row>
@@ -4945,7 +5437,7 @@
       <c r="E35" t="s">
         <v>311</v>
       </c>
-      <c r="R35" t="s">
+      <c r="S35" t="s">
         <v>123</v>
       </c>
     </row>
@@ -4953,7 +5445,7 @@
       <c r="E36" t="s">
         <v>265</v>
       </c>
-      <c r="R36" t="s">
+      <c r="S36" t="s">
         <v>342</v>
       </c>
     </row>
@@ -4961,7 +5453,7 @@
       <c r="E37" t="s">
         <v>312</v>
       </c>
-      <c r="R37" t="s">
+      <c r="S37" t="s">
         <v>406</v>
       </c>
     </row>
@@ -4969,7 +5461,7 @@
       <c r="E38" t="s">
         <v>271</v>
       </c>
-      <c r="R38" t="s">
+      <c r="S38" t="s">
         <v>124</v>
       </c>
     </row>
@@ -4977,7 +5469,7 @@
       <c r="E39" t="s">
         <v>80</v>
       </c>
-      <c r="R39" t="s">
+      <c r="S39" t="s">
         <v>125</v>
       </c>
     </row>
@@ -4985,7 +5477,7 @@
       <c r="E40" t="s">
         <v>216</v>
       </c>
-      <c r="R40" t="s">
+      <c r="S40" t="s">
         <v>126</v>
       </c>
     </row>
@@ -4993,7 +5485,7 @@
       <c r="E41" t="s">
         <v>293</v>
       </c>
-      <c r="R41" t="s">
+      <c r="S41" t="s">
         <v>127</v>
       </c>
     </row>
@@ -5001,7 +5493,7 @@
       <c r="E42" t="s">
         <v>304</v>
       </c>
-      <c r="R42" t="s">
+      <c r="S42" t="s">
         <v>128</v>
       </c>
     </row>
@@ -5009,7 +5501,7 @@
       <c r="E43" t="s">
         <v>305</v>
       </c>
-      <c r="R43" t="s">
+      <c r="S43" t="s">
         <v>129</v>
       </c>
     </row>
@@ -5017,7 +5509,7 @@
       <c r="E44" t="s">
         <v>347</v>
       </c>
-      <c r="R44" t="s">
+      <c r="S44" t="s">
         <v>217</v>
       </c>
     </row>
@@ -5025,7 +5517,7 @@
       <c r="E45" t="s">
         <v>346</v>
       </c>
-      <c r="R45" t="s">
+      <c r="S45" t="s">
         <v>79</v>
       </c>
     </row>
@@ -5033,7 +5525,7 @@
       <c r="E46" t="s">
         <v>215</v>
       </c>
-      <c r="R46" t="s">
+      <c r="S46" t="s">
         <v>130</v>
       </c>
     </row>
@@ -5041,7 +5533,7 @@
       <c r="E47" t="s">
         <v>324</v>
       </c>
-      <c r="R47" t="s">
+      <c r="S47" t="s">
         <v>131</v>
       </c>
     </row>
@@ -5049,7 +5541,7 @@
       <c r="E48" t="s">
         <v>343</v>
       </c>
-      <c r="R48" t="s">
+      <c r="S48" t="s">
         <v>132</v>
       </c>
     </row>
@@ -5057,7 +5549,7 @@
       <c r="E49" t="s">
         <v>374</v>
       </c>
-      <c r="R49" t="s">
+      <c r="S49" t="s">
         <v>133</v>
       </c>
     </row>
@@ -5065,7 +5557,7 @@
       <c r="E50" t="s">
         <v>306</v>
       </c>
-      <c r="R50" t="s">
+      <c r="S50" t="s">
         <v>350</v>
       </c>
     </row>
@@ -5073,412 +5565,409 @@
       <c r="E51" t="s">
         <v>360</v>
       </c>
-      <c r="R51" t="s">
+      <c r="S51" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="52">
       <c r="E52" t="s">
-        <v>361</v>
-      </c>
-      <c r="R52" t="s">
+        <v>335</v>
+      </c>
+      <c r="S52" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="53">
       <c r="E53" t="s">
-        <v>362</v>
-      </c>
-      <c r="R53" t="s">
+        <v>272</v>
+      </c>
+      <c r="S53" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="54">
       <c r="E54" t="s">
-        <v>335</v>
-      </c>
-      <c r="R54" t="s">
+        <v>296</v>
+      </c>
+      <c r="S54" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="55">
       <c r="E55" t="s">
-        <v>272</v>
-      </c>
-      <c r="R55" t="s">
+        <v>297</v>
+      </c>
+      <c r="S55" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="56">
       <c r="E56" t="s">
-        <v>296</v>
-      </c>
-      <c r="R56" t="s">
+        <v>298</v>
+      </c>
+      <c r="S56" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="57">
       <c r="E57" t="s">
-        <v>297</v>
-      </c>
-      <c r="R57" t="s">
+        <v>307</v>
+      </c>
+      <c r="S57" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="58">
       <c r="E58" t="s">
-        <v>298</v>
-      </c>
-      <c r="R58" t="s">
+        <v>316</v>
+      </c>
+      <c r="S58" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="59">
       <c r="E59" t="s">
-        <v>307</v>
-      </c>
-      <c r="R59" t="s">
+        <v>341</v>
+      </c>
+      <c r="S59" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="60">
       <c r="E60" t="s">
-        <v>316</v>
-      </c>
-      <c r="R60" t="s">
+        <v>313</v>
+      </c>
+      <c r="S60" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="61">
       <c r="E61" t="s">
-        <v>341</v>
-      </c>
-      <c r="R61" t="s">
+        <v>314</v>
+      </c>
+      <c r="S61" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="62">
       <c r="E62" t="s">
-        <v>313</v>
-      </c>
-      <c r="R62" t="s">
+        <v>375</v>
+      </c>
+      <c r="S62" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="63">
       <c r="E63" t="s">
-        <v>314</v>
-      </c>
-      <c r="R63" t="s">
+        <v>376</v>
+      </c>
+      <c r="S63" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="64">
       <c r="E64" t="s">
-        <v>375</v>
-      </c>
-      <c r="R64" t="s">
+        <v>349</v>
+      </c>
+      <c r="S64" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="65">
       <c r="E65" t="s">
-        <v>376</v>
-      </c>
-      <c r="R65" t="s">
+        <v>317</v>
+      </c>
+      <c r="S65" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="66">
       <c r="E66" t="s">
-        <v>349</v>
-      </c>
-      <c r="R66" t="s">
+        <v>273</v>
+      </c>
+      <c r="S66" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="67">
       <c r="E67" t="s">
-        <v>317</v>
-      </c>
-      <c r="R67" t="s">
+        <v>357</v>
+      </c>
+      <c r="S67" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="68">
       <c r="E68" t="s">
-        <v>273</v>
-      </c>
-      <c r="R68" t="s">
+        <v>318</v>
+      </c>
+      <c r="S68" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="69">
       <c r="E69" t="s">
-        <v>357</v>
-      </c>
-      <c r="R69" t="s">
+        <v>308</v>
+      </c>
+      <c r="S69" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="70">
       <c r="E70" t="s">
-        <v>318</v>
-      </c>
-      <c r="R70" t="s">
+        <v>416</v>
+      </c>
+      <c r="S70" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="71">
       <c r="E71" t="s">
-        <v>308</v>
-      </c>
-      <c r="R71" t="s">
+        <v>266</v>
+      </c>
+      <c r="S71" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="72">
       <c r="E72" t="s">
-        <v>266</v>
-      </c>
-      <c r="R72" t="s">
+        <v>348</v>
+      </c>
+      <c r="S72" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="73">
       <c r="E73" t="s">
-        <v>348</v>
-      </c>
-      <c r="R73" t="s">
+        <v>284</v>
+      </c>
+      <c r="S73" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="74">
       <c r="E74" t="s">
-        <v>284</v>
-      </c>
-      <c r="R74" t="s">
+        <v>290</v>
+      </c>
+      <c r="S74" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="75">
       <c r="E75" t="s">
-        <v>290</v>
-      </c>
-      <c r="R75" t="s">
+        <v>295</v>
+      </c>
+      <c r="S75" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="76">
       <c r="E76" t="s">
-        <v>295</v>
-      </c>
-      <c r="R76" t="s">
+        <v>336</v>
+      </c>
+      <c r="S76" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="77">
       <c r="E77" t="s">
-        <v>336</v>
-      </c>
-      <c r="R77" t="s">
+        <v>274</v>
+      </c>
+      <c r="S77" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="78">
       <c r="E78" t="s">
-        <v>274</v>
-      </c>
-      <c r="R78" t="s">
+        <v>285</v>
+      </c>
+      <c r="S78" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="79">
       <c r="E79" t="s">
-        <v>285</v>
-      </c>
-      <c r="R79" t="s">
+        <v>291</v>
+      </c>
+      <c r="S79" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="80">
       <c r="E80" t="s">
-        <v>291</v>
-      </c>
-      <c r="R80" t="s">
+        <v>280</v>
+      </c>
+      <c r="S80" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="81">
       <c r="E81" t="s">
-        <v>280</v>
-      </c>
-      <c r="R81" t="s">
+        <v>275</v>
+      </c>
+      <c r="S81" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="82">
       <c r="E82" t="s">
-        <v>275</v>
-      </c>
-      <c r="R82" t="s">
+        <v>292</v>
+      </c>
+      <c r="S82" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="83">
       <c r="E83" t="s">
-        <v>292</v>
-      </c>
-      <c r="R83" t="s">
+        <v>276</v>
+      </c>
+      <c r="S83" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="84">
       <c r="E84" t="s">
-        <v>276</v>
-      </c>
-      <c r="R84" t="s">
+        <v>277</v>
+      </c>
+      <c r="S84" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="85">
       <c r="E85" t="s">
-        <v>277</v>
-      </c>
-      <c r="R85" t="s">
+        <v>309</v>
+      </c>
+      <c r="S85" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="86">
       <c r="E86" t="s">
-        <v>309</v>
-      </c>
-      <c r="R86" t="s">
+        <v>315</v>
+      </c>
+      <c r="S86" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="87">
       <c r="E87" t="s">
-        <v>315</v>
-      </c>
-      <c r="R87" t="s">
+        <v>299</v>
+      </c>
+      <c r="S87" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="88">
       <c r="E88" t="s">
-        <v>299</v>
-      </c>
-      <c r="R88" t="s">
+        <v>344</v>
+      </c>
+      <c r="S88" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="89">
       <c r="E89" t="s">
-        <v>344</v>
-      </c>
-      <c r="R89" t="s">
+        <v>281</v>
+      </c>
+      <c r="S89" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="90">
       <c r="E90" t="s">
-        <v>281</v>
-      </c>
-      <c r="R90" t="s">
+        <v>282</v>
+      </c>
+      <c r="S90" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="91">
-      <c r="E91" t="s">
-        <v>282</v>
-      </c>
-      <c r="R91" t="s">
+      <c r="S91" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="92">
-      <c r="R92" t="s">
+      <c r="S92" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="93">
-      <c r="R93" t="s">
+      <c r="S93" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="94">
-      <c r="R94" t="s">
+      <c r="S94" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="95">
-      <c r="R95" t="s">
+      <c r="S95" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="96">
-      <c r="R96" t="s">
+      <c r="S96" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="97">
-      <c r="R97" t="s">
+      <c r="S97" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="98">
-      <c r="R98" t="s">
+      <c r="S98" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="99">
-      <c r="R99" t="s">
+      <c r="S99" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="100">
-      <c r="R100" t="s">
+      <c r="S100" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="101">
-      <c r="R101" t="s">
+      <c r="S101" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="102">
-      <c r="R102" t="s">
+      <c r="S102" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="103">
-      <c r="R103" t="s">
+      <c r="S103" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="104">
-      <c r="R104" t="s">
+      <c r="S104" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="105">
-      <c r="R105" t="s">
+      <c r="S105" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="106">
-      <c r="R106" t="s">
+      <c r="S106" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="107">
-      <c r="R107" t="s">
+      <c r="S107" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="108">
-      <c r="R108" t="s">
+      <c r="S108" t="s">
         <v>173</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- update command listing - new example: craigslist
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/script/rdbms-01.xlsx
+++ b/artifact/script/rdbms-01.xlsx
@@ -18,40 +18,41 @@
   </sheets>
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
-    <definedName name="base">'#system'!$E$2:$E$39</definedName>
-    <definedName name="csv">'#system'!$F$2:$F$6</definedName>
+    <definedName name="base">'#system'!$F$2:$F$40</definedName>
+    <definedName name="csv">'#system'!$G$2:$G$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$G$2:$G$98</definedName>
-    <definedName name="excel">'#system'!$H$2:$H$14</definedName>
-    <definedName name="external">'#system'!$I$2:$I$5</definedName>
-    <definedName name="image">'#system'!$J$2:$J$7</definedName>
-    <definedName name="io">'#system'!$K$2:$K$29</definedName>
-    <definedName name="jms">'#system'!$L$2:$L$4</definedName>
-    <definedName name="json">'#system'!$M$2:$M$18</definedName>
-    <definedName name="mail">'#system'!$P$2:$P$2</definedName>
+    <definedName name="desktop">'#system'!$H$2:$H$98</definedName>
+    <definedName name="excel">'#system'!$I$2:$I$14</definedName>
+    <definedName name="external">'#system'!$J$2:$J$5</definedName>
+    <definedName name="image">'#system'!$K$2:$K$7</definedName>
+    <definedName name="io">'#system'!$L$2:$L$30</definedName>
+    <definedName name="jms">'#system'!$M$2:$M$4</definedName>
+    <definedName name="json">'#system'!$N$2:$N$18</definedName>
+    <definedName name="mail">'#system'!$Q$2:$Q$2</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
-    <definedName name="number">'#system'!$Q$2:$Q$16</definedName>
-    <definedName name="pdf">'#system'!$R$2:$R$16</definedName>
-    <definedName name="rdbms">'#system'!$S$2:$S$7</definedName>
-    <definedName name="redis">'#system'!$T$2:$T$10</definedName>
-    <definedName name="sms">'#system'!$U$2:$U$2</definedName>
-    <definedName name="sound">'#system'!$V$2:$V$5</definedName>
-    <definedName name="ssh">'#system'!$W$2:$W$9</definedName>
-    <definedName name="step">'#system'!$X$2:$X$4</definedName>
-    <definedName name="target">'#system'!$A$2:$A$30</definedName>
-    <definedName name="web">'#system'!$Y$2:$Y$134</definedName>
-    <definedName name="webalert">'#system'!$Z$2:$Z$8</definedName>
-    <definedName name="webcookie">'#system'!$AA$2:$AA$8</definedName>
-    <definedName name="ws">'#system'!$AB$2:$AB$17</definedName>
-    <definedName name="ws.async">'#system'!$AC$2:$AC$8</definedName>
-    <definedName name="xml">'#system'!$AD$2:$AD$27</definedName>
+    <definedName name="number">'#system'!$R$2:$R$16</definedName>
+    <definedName name="pdf">'#system'!$S$2:$S$16</definedName>
+    <definedName name="rdbms">'#system'!$T$2:$T$7</definedName>
+    <definedName name="redis">'#system'!$U$2:$U$10</definedName>
+    <definedName name="sms">'#system'!$V$2:$V$2</definedName>
+    <definedName name="sound">'#system'!$W$2:$W$5</definedName>
+    <definedName name="ssh">'#system'!$X$2:$X$9</definedName>
+    <definedName name="step">'#system'!$Y$2:$Y$4</definedName>
+    <definedName name="target">'#system'!$A$2:$A$31</definedName>
+    <definedName name="web">'#system'!$Z$2:$Z$135</definedName>
+    <definedName name="webalert">'#system'!$AA$2:$AA$8</definedName>
+    <definedName name="webcookie">'#system'!$AB$2:$AB$8</definedName>
+    <definedName name="ws">'#system'!$AC$2:$AC$17</definedName>
+    <definedName name="ws.async">'#system'!$AD$2:$AD$8</definedName>
+    <definedName name="xml">'#system'!$AE$2:$AE$27</definedName>
     <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
-    <definedName name="macro">'#system'!$O$2:$O$4</definedName>
+    <definedName name="macro">'#system'!$P$2:$P$4</definedName>
     <definedName name="aws.sqs">'#system'!$D$2:$D$6</definedName>
-    <definedName name="localdb">'#system'!$N$2:$N$12</definedName>
+    <definedName name="localdb">'#system'!$O$2:$O$12</definedName>
+    <definedName name="aws.vision">'#system'!$E$2:$E$2</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14763" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15888" uniqueCount="572">
   <si>
     <t>description</t>
   </si>
@@ -1762,13 +1763,46 @@
   <si>
     <t>storeSoapFaultString(var,xml)</t>
   </si>
+  <si>
+    <t>aws.vision</t>
+  </si>
+  <si>
+    <t>saveText(profile,image,var)</t>
+  </si>
+  <si>
+    <t>assertNotContain(text,substring)</t>
+  </si>
+  <si>
+    <t>clear(variables)</t>
+  </si>
+  <si>
+    <t>saveMatches(var,path,fileFilter,textFilter)</t>
+  </si>
+  <si>
+    <t>assertAttributeNotContain(locator,attrName,contains)</t>
+  </si>
+  <si>
+    <t>assertTextNotContain(locator,text)</t>
+  </si>
+  <si>
+    <t>screenshot(file,locator)</t>
+  </si>
+  <si>
+    <t>clearVariables(variables)</t>
+  </si>
+  <si>
+    <t>assertPath(path)</t>
+  </si>
+  <si>
+    <t>assertAttributeContain(locator,attrName,contains)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="464" x14ac:knownFonts="1">
+  <fonts count="496" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4697,8 +4731,210 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="808">
+  <fills count="862">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -9273,8 +9509,314 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="819">
+  <borders count="883">
     <border>
       <left/>
       <right/>
@@ -17030,6 +17572,658 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -17541,7 +18735,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="489">
+  <cellXfs count="521">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -18978,52 +20172,148 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="780" fontId="447" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="448" fillId="783" borderId="794" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="794" fillId="783" fontId="448" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="449" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="449" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="450" fillId="786" borderId="798" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="798" fillId="786" fontId="450" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="451" fillId="789" borderId="802" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="802" fillId="789" fontId="451" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="452" fillId="792" borderId="806" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="806" fillId="792" fontId="452" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="453" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="453" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="454" fillId="795" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="795" fontId="454" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="455" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="455" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="456" fillId="798" borderId="810" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="810" fillId="798" fontId="456" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="457" fillId="789" borderId="814" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="814" fillId="789" fontId="457" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="458" fillId="801" borderId="818" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="818" fillId="801" fontId="458" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="459" fillId="801" borderId="818" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="818" fillId="801" fontId="459" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="460" fillId="792" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="792" fontId="460" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="461" fillId="804" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="804" fontId="461" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="462" fillId="792" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="792" fontId="462" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="463" fillId="807" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="807" fontId="463" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="826" fillId="810" fontId="464" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="465" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="830" fillId="813" fontId="466" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="834" fillId="816" fontId="467" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="838" fillId="819" fontId="468" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="469" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="822" fontId="470" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="471" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="842" fillId="825" fontId="472" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="846" fillId="816" fontId="473" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="850" fillId="828" fontId="474" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="850" fillId="828" fontId="475" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="819" fontId="476" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="831" fontId="477" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="819" fontId="478" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="834" fontId="479" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="480" fillId="837" borderId="858" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="481" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="482" fillId="840" borderId="862" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="483" fillId="843" borderId="866" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="484" fillId="846" borderId="870" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="485" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="486" fillId="849" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="487" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="488" fillId="852" borderId="874" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="489" fillId="843" borderId="878" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="490" fillId="855" borderId="882" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="491" fillId="855" borderId="882" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="492" fillId="846" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="493" fillId="858" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="494" fillId="846" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="495" fillId="861" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -19348,7 +20638,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE134"/>
+  <dimension ref="A1:AF135"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
       <selection activeCell="A19" sqref="A19"/>
@@ -19373,81 +20663,84 @@
         <v>497</v>
       </c>
       <c r="E1" t="s">
+        <v>561</v>
+      </c>
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>51</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>347</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>333</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>24</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>523</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>483</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>196</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>52</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>239</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>53</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>407</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>431</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>421</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>357</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>403</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>54</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>55</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>56</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>57</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>432</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>227</v>
       </c>
     </row>
@@ -19465,81 +20758,84 @@
         <v>498</v>
       </c>
       <c r="E2" t="s">
+        <v>562</v>
+      </c>
+      <c r="F2" t="s">
         <v>58</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>72</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>74</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>460</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>79</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>478</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>315</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>384</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>434</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>524</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>488</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>424</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>435</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>253</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>217</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>409</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>438</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>426</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>381</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>404</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>97</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>171</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>176</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>183</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>440</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>502</v>
       </c>
     </row>
@@ -19556,76 +20852,76 @@
       <c r="D3" t="s">
         <v>534</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>469</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>365</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>88</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>49</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>484</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>349</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>341</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>334</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>86</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>525</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>489</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>436</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>240</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>218</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>410</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>427</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>382</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>405</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>98</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>172</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>177</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>364</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>184</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>228</v>
       </c>
     </row>
@@ -19639,82 +20935,82 @@
       <c r="D4" t="s">
         <v>499</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>73</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>387</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>461</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>485</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>350</v>
       </c>
-      <c r="K4" t="s">
-        <v>238</v>
-      </c>
       <c r="L4" t="s">
+        <v>570</v>
+      </c>
+      <c r="M4" t="s">
         <v>335</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>25</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>526</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>490</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>26</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>241</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>219</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>411</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>428</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>358</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>406</v>
       </c>
-      <c r="Y4" t="s">
-        <v>354</v>
-      </c>
       <c r="Z4" t="s">
+        <v>571</v>
+      </c>
+      <c r="AA4" t="s">
         <v>173</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>178</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>184</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>441</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>561</v>
       </c>
       <c r="B5" t="s">
         <v>375</v>
@@ -19722,73 +21018,73 @@
       <c r="D5" t="s">
         <v>500</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>470</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>451</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>539</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>467</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>544</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>351</v>
       </c>
-      <c r="K5" t="s">
-        <v>475</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="L5" t="s">
+        <v>238</v>
+      </c>
+      <c r="N5" t="s">
         <v>87</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>536</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>30</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>242</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>220</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>412</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>429</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>359</v>
       </c>
-      <c r="Y5" t="s">
-        <v>355</v>
-      </c>
       <c r="Z5" t="s">
+        <v>566</v>
+      </c>
+      <c r="AA5" t="s">
         <v>174</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>179</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>185</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>442</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>376</v>
@@ -19796,1505 +21092,1519 @@
       <c r="D6" t="s">
         <v>501</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>27</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>514</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>336</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>462</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>348</v>
       </c>
-      <c r="K6" t="s">
-        <v>72</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="L6" t="s">
+        <v>475</v>
+      </c>
+      <c r="N6" t="s">
         <v>29</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>530</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>31</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>243</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>391</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>413</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>361</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>99</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>455</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>180</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>186</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>443</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
         <v>377</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>224</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>388</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>458</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>545</v>
       </c>
-      <c r="K7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="L7" t="s">
+        <v>72</v>
+      </c>
+      <c r="N7" t="s">
         <v>315</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>531</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>33</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>244</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>425</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>414</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>360</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>100</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>456</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>181</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>187</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>444</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>555</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>378</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>318</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>366</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>328</v>
       </c>
-      <c r="K8" t="s">
-        <v>517</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="L8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" t="s">
         <v>34</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>532</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>91</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>245</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>415</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>362</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>101</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>175</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>182</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AC8" t="s">
         <v>188</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>445</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AE8" t="s">
         <v>556</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>379</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>32</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>367</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>329</v>
       </c>
-      <c r="K9" t="s">
-        <v>80</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="L9" t="s">
+        <v>517</v>
+      </c>
+      <c r="N9" t="s">
         <v>35</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>537</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>92</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>246</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>416</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>363</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="Z9" t="s">
         <v>209</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AC9" t="s">
         <v>189</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AE9" t="s">
         <v>557</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>347</v>
-      </c>
-      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
         <v>315</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>306</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>463</v>
       </c>
-      <c r="K10" t="s">
-        <v>38</v>
-      </c>
-      <c r="M10" t="s">
+      <c r="L10" t="s">
+        <v>80</v>
+      </c>
+      <c r="N10" t="s">
         <v>36</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>527</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>437</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>247</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>417</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="Z10" t="s">
         <v>257</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AC10" t="s">
         <v>190</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AE10" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" t="s">
-        <v>255</v>
-      </c>
-      <c r="G11" t="s">
+        <v>347</v>
+      </c>
+      <c r="F11" t="s">
+        <v>563</v>
+      </c>
+      <c r="H11" t="s">
         <v>352</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>322</v>
       </c>
-      <c r="K11" t="s">
-        <v>518</v>
-      </c>
-      <c r="M11" t="s">
+      <c r="L11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N11" t="s">
         <v>486</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>528</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>93</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>248</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="Z11" t="s">
         <v>258</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC11" t="s">
         <v>259</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AE11" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>333</v>
-      </c>
-      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
         <v>319</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>274</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>323</v>
       </c>
-      <c r="K12" t="s">
-        <v>390</v>
-      </c>
-      <c r="M12" t="s">
+      <c r="L12" t="s">
+        <v>518</v>
+      </c>
+      <c r="N12" t="s">
         <v>546</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>529</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>41</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>249</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="Z12" t="s">
         <v>102</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AC12" t="s">
         <v>191</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AE12" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" t="s">
+        <v>333</v>
+      </c>
+      <c r="F13" t="s">
         <v>341</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>263</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>324</v>
       </c>
-      <c r="K13" t="s">
-        <v>17</v>
-      </c>
-      <c r="M13" t="s">
+      <c r="L13" t="s">
+        <v>390</v>
+      </c>
+      <c r="N13" t="s">
         <v>453</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>94</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>254</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="Z13" t="s">
         <v>326</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AC13" t="s">
         <v>192</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AE13" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>523</v>
-      </c>
-      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
         <v>37</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>316</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>325</v>
       </c>
-      <c r="K14" t="s">
-        <v>42</v>
-      </c>
-      <c r="M14" t="s">
+      <c r="L14" t="s">
+        <v>17</v>
+      </c>
+      <c r="N14" t="s">
         <v>487</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>95</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>250</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="Z14" t="s">
         <v>103</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AC14" t="s">
         <v>193</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AE14" t="s">
         <v>503</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>483</v>
-      </c>
-      <c r="E15" t="s">
+        <v>523</v>
+      </c>
+      <c r="F15" t="s">
         <v>59</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>264</v>
       </c>
-      <c r="K15" t="s">
-        <v>519</v>
-      </c>
-      <c r="M15" t="s">
+      <c r="L15" t="s">
+        <v>42</v>
+      </c>
+      <c r="N15" t="s">
         <v>39</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>511</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>251</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="Z15" t="s">
         <v>104</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AC15" t="s">
         <v>194</v>
       </c>
-      <c r="AD15" t="s">
+      <c r="AE15" t="s">
         <v>504</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>196</v>
-      </c>
-      <c r="E16" t="s">
+        <v>483</v>
+      </c>
+      <c r="F16" t="s">
         <v>385</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>265</v>
       </c>
-      <c r="K16" t="s">
-        <v>81</v>
-      </c>
-      <c r="M16" t="s">
+      <c r="L16" t="s">
+        <v>519</v>
+      </c>
+      <c r="N16" t="s">
         <v>547</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>512</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>252</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="Z16" t="s">
         <v>75</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AC16" t="s">
         <v>195</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AE16" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" t="s">
+        <v>196</v>
+      </c>
+      <c r="F17" t="s">
         <v>386</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>317</v>
       </c>
-      <c r="K17" t="s">
-        <v>82</v>
-      </c>
-      <c r="M17" t="s">
+      <c r="L17" t="s">
+        <v>81</v>
+      </c>
+      <c r="N17" t="s">
         <v>40</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="Z17" t="s">
         <v>513</v>
       </c>
-      <c r="AB17" t="s">
+      <c r="AC17" t="s">
         <v>477</v>
       </c>
-      <c r="AD17" t="s">
+      <c r="AE17" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>239</v>
-      </c>
-      <c r="E18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" t="s">
         <v>422</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>89</v>
       </c>
-      <c r="K18" t="s">
-        <v>468</v>
-      </c>
-      <c r="M18" t="s">
+      <c r="L18" t="s">
+        <v>82</v>
+      </c>
+      <c r="N18" t="s">
         <v>43</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="Z18" t="s">
         <v>105</v>
       </c>
-      <c r="AD18" t="s">
+      <c r="AE18" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G19" t="s">
+        <v>239</v>
+      </c>
+      <c r="F19" t="s">
+        <v>569</v>
+      </c>
+      <c r="H19" t="s">
         <v>90</v>
       </c>
-      <c r="K19" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y19" t="s">
+      <c r="L19" t="s">
+        <v>468</v>
+      </c>
+      <c r="Z19" t="s">
         <v>106</v>
       </c>
-      <c r="AD19" t="s">
+      <c r="AE19" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>407</v>
-      </c>
-      <c r="E20" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" t="s">
         <v>296</v>
       </c>
-      <c r="K20" t="s">
-        <v>84</v>
-      </c>
-      <c r="Y20" t="s">
+      <c r="L20" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z20" t="s">
         <v>107</v>
       </c>
-      <c r="AD20" t="s">
+      <c r="AE20" t="s">
         <v>506</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>431</v>
-      </c>
-      <c r="E21" t="s">
-        <v>256</v>
-      </c>
-      <c r="G21" t="s">
+        <v>407</v>
+      </c>
+      <c r="F21" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" t="s">
         <v>297</v>
       </c>
-      <c r="K21" t="s">
-        <v>380</v>
-      </c>
-      <c r="Y21" t="s">
+      <c r="L21" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z21" t="s">
         <v>108</v>
       </c>
-      <c r="AD21" t="s">
+      <c r="AE21" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>421</v>
-      </c>
-      <c r="E22" t="s">
-        <v>538</v>
-      </c>
-      <c r="G22" t="s">
+        <v>431</v>
+      </c>
+      <c r="F22" t="s">
+        <v>256</v>
+      </c>
+      <c r="H22" t="s">
         <v>298</v>
       </c>
-      <c r="K22" t="s">
-        <v>482</v>
-      </c>
-      <c r="Y22" t="s">
+      <c r="L22" t="s">
+        <v>565</v>
+      </c>
+      <c r="Z22" t="s">
         <v>491</v>
       </c>
-      <c r="AD22" t="s">
+      <c r="AE22" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>357</v>
-      </c>
-      <c r="E23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G23" t="s">
+        <v>421</v>
+      </c>
+      <c r="F23" t="s">
+        <v>538</v>
+      </c>
+      <c r="H23" t="s">
         <v>299</v>
       </c>
-      <c r="K23" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y23" t="s">
+      <c r="L23" t="s">
+        <v>482</v>
+      </c>
+      <c r="Z23" t="s">
         <v>110</v>
       </c>
-      <c r="AD23" t="s">
+      <c r="AE23" t="s">
         <v>558</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>403</v>
-      </c>
-      <c r="E24" t="s">
-        <v>321</v>
-      </c>
-      <c r="G24" t="s">
+        <v>357</v>
+      </c>
+      <c r="F24" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" t="s">
         <v>290</v>
       </c>
-      <c r="K24" t="s">
-        <v>399</v>
-      </c>
-      <c r="Y24" t="s">
+      <c r="L24" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z24" t="s">
         <v>548</v>
       </c>
-      <c r="AD24" t="s">
+      <c r="AE24" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" t="s">
+        <v>403</v>
+      </c>
+      <c r="F25" t="s">
+        <v>321</v>
+      </c>
+      <c r="H25" t="s">
         <v>279</v>
       </c>
-      <c r="K25" t="s">
-        <v>535</v>
-      </c>
-      <c r="Y25" t="s">
+      <c r="L25" t="s">
+        <v>399</v>
+      </c>
+      <c r="Z25" t="s">
         <v>111</v>
       </c>
-      <c r="AD25" t="s">
+      <c r="AE25" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26" t="s">
-        <v>459</v>
-      </c>
-      <c r="G26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" t="s">
+        <v>63</v>
+      </c>
+      <c r="H26" t="s">
         <v>76</v>
       </c>
-      <c r="K26" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y26" t="s">
+      <c r="L26" t="s">
+        <v>535</v>
+      </c>
+      <c r="Z26" t="s">
         <v>112</v>
       </c>
-      <c r="AD26" t="s">
+      <c r="AE26" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" t="s">
-        <v>225</v>
-      </c>
-      <c r="G27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" t="s">
+        <v>459</v>
+      </c>
+      <c r="H27" t="s">
         <v>282</v>
       </c>
-      <c r="K27" t="s">
-        <v>452</v>
-      </c>
-      <c r="Y27" t="s">
+      <c r="L27" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z27" t="s">
         <v>113</v>
       </c>
-      <c r="AD27" t="s">
+      <c r="AE27" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>57</v>
-      </c>
-      <c r="E28" t="s">
-        <v>226</v>
-      </c>
-      <c r="G28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" t="s">
+        <v>225</v>
+      </c>
+      <c r="H28" t="s">
         <v>266</v>
       </c>
-      <c r="K28" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y28" t="s">
+      <c r="L28" t="s">
+        <v>452</v>
+      </c>
+      <c r="Z28" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>432</v>
-      </c>
-      <c r="E29" t="s">
-        <v>479</v>
-      </c>
-      <c r="G29" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" t="s">
+        <v>226</v>
+      </c>
+      <c r="H29" t="s">
         <v>283</v>
       </c>
-      <c r="K29" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y29" t="s">
+      <c r="L29" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z29" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>432</v>
+      </c>
+      <c r="F30" t="s">
+        <v>479</v>
+      </c>
+      <c r="H30" t="s">
+        <v>284</v>
+      </c>
+      <c r="L30" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
         <v>227</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F31" t="s">
         <v>480</v>
       </c>
-      <c r="G30" t="s">
-        <v>284</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="E31" t="s">
+      <c r="H31" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="F32" t="s">
         <v>430</v>
       </c>
-      <c r="G31" t="s">
-        <v>216</v>
-      </c>
-      <c r="Y31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="E32" t="s">
+      <c r="H32" t="s">
+        <v>275</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="F33" t="s">
         <v>64</v>
       </c>
-      <c r="G32" t="s">
-        <v>275</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="E33" t="s">
+      <c r="H33" t="s">
+        <v>285</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="F34" t="s">
         <v>65</v>
       </c>
-      <c r="G33" t="s">
-        <v>285</v>
-      </c>
-      <c r="Y33" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="E34" t="s">
+      <c r="H34" t="s">
+        <v>515</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="F35" t="s">
         <v>66</v>
       </c>
-      <c r="G34" t="s">
-        <v>515</v>
-      </c>
-      <c r="Y34" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="E35" t="s">
+      <c r="H35" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="F36" t="s">
         <v>67</v>
       </c>
-      <c r="G35" t="s">
-        <v>260</v>
-      </c>
-      <c r="Y35" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="E36" t="s">
+      <c r="H36" t="s">
+        <v>330</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="F37" t="s">
         <v>68</v>
       </c>
-      <c r="G36" t="s">
-        <v>330</v>
-      </c>
-      <c r="Y36" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="E37" t="s">
+      <c r="H37" t="s">
+        <v>307</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="F38" t="s">
         <v>69</v>
       </c>
-      <c r="G37" t="s">
-        <v>307</v>
-      </c>
-      <c r="Y37" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="E38" t="s">
+      <c r="H38" t="s">
+        <v>261</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="F39" t="s">
         <v>70</v>
       </c>
-      <c r="G38" t="s">
-        <v>261</v>
-      </c>
-      <c r="Y38" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="E39" t="s">
+      <c r="H39" t="s">
+        <v>308</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="F40" t="s">
         <v>71</v>
       </c>
-      <c r="G39" t="s">
-        <v>308</v>
-      </c>
-      <c r="Y39" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>267</v>
       </c>
-      <c r="Y40" t="s">
+      <c r="Z40" t="s">
         <v>439</v>
       </c>
     </row>
     <row r="41">
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>78</v>
       </c>
-      <c r="Y41" t="s">
-        <v>550</v>
+      <c r="Z41" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="42">
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>212</v>
       </c>
-      <c r="Y42" t="s">
+      <c r="Z42" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="43">
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>540</v>
       </c>
-      <c r="Y43" t="s">
+      <c r="Z43" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="44">
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>289</v>
       </c>
-      <c r="Y44" t="s">
+      <c r="Z44" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="45">
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>300</v>
       </c>
-      <c r="Y45" t="s">
+      <c r="Z45" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="46">
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>301</v>
       </c>
-      <c r="Y46" t="s">
+      <c r="Z46" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="47">
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>343</v>
       </c>
-      <c r="Y47" t="s">
+      <c r="Z47" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="48">
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>342</v>
       </c>
-      <c r="Y48" t="s">
+      <c r="Z48" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="49">
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>211</v>
       </c>
-      <c r="Y49" t="s">
+      <c r="Z49" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="50">
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>320</v>
       </c>
-      <c r="Y50" t="s">
+      <c r="Z50" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="51">
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>339</v>
       </c>
-      <c r="Y51" t="s">
+      <c r="Z51" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="52">
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>368</v>
       </c>
-      <c r="Y52" t="s">
+      <c r="Z52" t="s">
         <v>551</v>
       </c>
     </row>
     <row r="53">
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>302</v>
       </c>
-      <c r="Y53" t="s">
+      <c r="Z53" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="54">
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>356</v>
       </c>
-      <c r="Y54" t="s">
+      <c r="Z54" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="55">
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>331</v>
       </c>
-      <c r="Y55" t="s">
+      <c r="Z55" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="56">
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>268</v>
       </c>
-      <c r="Y56" t="s">
+      <c r="Z56" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="57">
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>292</v>
       </c>
-      <c r="Y57" t="s">
+      <c r="Z57" t="s">
         <v>476</v>
       </c>
     </row>
     <row r="58">
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>293</v>
       </c>
-      <c r="Y58" t="s">
+      <c r="Z58" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="59">
-      <c r="G59" t="s">
+      <c r="H59" t="s">
         <v>541</v>
       </c>
-      <c r="Y59" t="s">
+      <c r="Z59" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="60">
-      <c r="G60" t="s">
+      <c r="H60" t="s">
         <v>294</v>
       </c>
-      <c r="Y60" t="s">
+      <c r="Z60" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="61">
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>303</v>
       </c>
-      <c r="Y61" t="s">
+      <c r="Z61" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="62">
-      <c r="G62" t="s">
+      <c r="H62" t="s">
         <v>312</v>
       </c>
-      <c r="Y62" t="s">
+      <c r="Z62" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="63">
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>337</v>
       </c>
-      <c r="Y63" t="s">
+      <c r="Z63" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="64">
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>309</v>
       </c>
-      <c r="Y64" t="s">
+      <c r="Z64" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="65">
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>310</v>
       </c>
-      <c r="Y65" t="s">
+      <c r="Z65" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="66">
-      <c r="G66" t="s">
+      <c r="H66" t="s">
         <v>369</v>
       </c>
-      <c r="Y66" t="s">
+      <c r="Z66" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="67">
-      <c r="G67" t="s">
+      <c r="H67" t="s">
         <v>370</v>
       </c>
-      <c r="Y67" t="s">
+      <c r="Z67" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="68">
-      <c r="G68" t="s">
+      <c r="H68" t="s">
         <v>345</v>
       </c>
-      <c r="Y68" t="s">
+      <c r="Z68" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="69">
-      <c r="G69" t="s">
+      <c r="H69" t="s">
         <v>313</v>
       </c>
-      <c r="Y69" t="s">
+      <c r="Z69" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="70">
-      <c r="G70" t="s">
+      <c r="H70" t="s">
         <v>269</v>
       </c>
-      <c r="Y70" t="s">
+      <c r="Z70" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="71">
-      <c r="G71" t="s">
+      <c r="H71" t="s">
         <v>542</v>
       </c>
-      <c r="Y71" t="s">
+      <c r="Z71" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="72">
-      <c r="G72" t="s">
+      <c r="H72" t="s">
         <v>314</v>
       </c>
-      <c r="Y72" t="s">
+      <c r="Z72" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="73">
-      <c r="G73" t="s">
+      <c r="H73" t="s">
         <v>423</v>
       </c>
-      <c r="Y73" t="s">
+      <c r="Z73" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="74">
-      <c r="G74" t="s">
+      <c r="H74" t="s">
         <v>304</v>
       </c>
-      <c r="Y74" t="s">
+      <c r="Z74" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="75">
-      <c r="G75" t="s">
+      <c r="H75" t="s">
         <v>408</v>
       </c>
-      <c r="Y75" t="s">
+      <c r="Z75" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="76">
-      <c r="G76" t="s">
+      <c r="H76" t="s">
         <v>262</v>
       </c>
-      <c r="Y76" t="s">
+      <c r="Z76" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="77">
-      <c r="G77" t="s">
+      <c r="H77" t="s">
         <v>516</v>
       </c>
-      <c r="Y77" t="s">
+      <c r="Z77" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="78">
-      <c r="G78" t="s">
+      <c r="H78" t="s">
         <v>344</v>
       </c>
-      <c r="Y78" t="s">
+      <c r="Z78" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="79">
-      <c r="G79" t="s">
+      <c r="H79" t="s">
         <v>280</v>
       </c>
-      <c r="Y79" t="s">
+      <c r="Z79" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="80">
-      <c r="G80" t="s">
+      <c r="H80" t="s">
         <v>286</v>
       </c>
-      <c r="Y80" t="s">
+      <c r="Z80" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="81">
-      <c r="G81" t="s">
+      <c r="H81" t="s">
         <v>291</v>
       </c>
-      <c r="Y81" t="s">
+      <c r="Z81" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="82">
-      <c r="G82" t="s">
+      <c r="H82" t="s">
         <v>433</v>
       </c>
-      <c r="Y82" t="s">
+      <c r="Z82" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="83">
-      <c r="G83" t="s">
+      <c r="H83" t="s">
         <v>332</v>
       </c>
-      <c r="Y83" t="s">
+      <c r="Z83" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="84">
-      <c r="G84" t="s">
+      <c r="H84" t="s">
         <v>270</v>
       </c>
-      <c r="Y84" t="s">
+      <c r="Z84" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="85">
-      <c r="G85" t="s">
+      <c r="H85" t="s">
         <v>281</v>
       </c>
-      <c r="Y85" t="s">
+      <c r="Z85" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="86">
-      <c r="G86" t="s">
+      <c r="H86" t="s">
         <v>287</v>
       </c>
-      <c r="Y86" t="s">
+      <c r="Z86" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="87">
-      <c r="G87" t="s">
+      <c r="H87" t="s">
         <v>276</v>
       </c>
-      <c r="Y87" t="s">
+      <c r="Z87" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="88">
-      <c r="G88" t="s">
+      <c r="H88" t="s">
         <v>543</v>
       </c>
-      <c r="Y88" t="s">
+      <c r="Z88" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="89">
-      <c r="G89" t="s">
+      <c r="H89" t="s">
         <v>271</v>
       </c>
-      <c r="Y89" t="s">
+      <c r="Z89" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="90">
-      <c r="G90" t="s">
+      <c r="H90" t="s">
         <v>288</v>
       </c>
-      <c r="Y90" t="s">
+      <c r="Z90" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="91">
-      <c r="G91" t="s">
+      <c r="H91" t="s">
         <v>272</v>
       </c>
-      <c r="Y91" t="s">
+      <c r="Z91" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="92">
-      <c r="G92" t="s">
+      <c r="H92" t="s">
         <v>273</v>
       </c>
-      <c r="Y92" t="s">
+      <c r="Z92" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="93">
-      <c r="G93" t="s">
+      <c r="H93" t="s">
         <v>305</v>
       </c>
-      <c r="Y93" t="s">
+      <c r="Z93" t="s">
         <v>552</v>
       </c>
     </row>
     <row r="94">
-      <c r="G94" t="s">
+      <c r="H94" t="s">
         <v>311</v>
       </c>
-      <c r="Y94" t="s">
+      <c r="Z94" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="95">
-      <c r="G95" t="s">
+      <c r="H95" t="s">
         <v>295</v>
       </c>
-      <c r="Y95" t="s">
+      <c r="Z95" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="96">
-      <c r="G96" t="s">
+      <c r="H96" t="s">
         <v>340</v>
       </c>
-      <c r="Y96" t="s">
+      <c r="Z96" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="97">
-      <c r="G97" t="s">
+      <c r="H97" t="s">
         <v>277</v>
       </c>
-      <c r="Y97" t="s">
+      <c r="Z97" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="98">
-      <c r="G98" t="s">
+      <c r="H98" t="s">
         <v>278</v>
       </c>
-      <c r="Y98" t="s">
+      <c r="Z98" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="99">
-      <c r="Y99" t="s">
+      <c r="Z99" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="100">
-      <c r="Y100" t="s">
+      <c r="Z100" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="101">
-      <c r="Y101" t="s">
+      <c r="Z101" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="102">
-      <c r="Y102" t="s">
+      <c r="Z102" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="103">
-      <c r="Y103" t="s">
+      <c r="Z103" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="104">
-      <c r="Y104" t="s">
+      <c r="Z104" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="105">
-      <c r="Y105" t="s">
+      <c r="Z105" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="106">
-      <c r="Y106" t="s">
+      <c r="Z106" t="s">
         <v>520</v>
       </c>
     </row>
     <row r="107">
-      <c r="Y107" t="s">
+      <c r="Z107" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="Z108" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="108">
-      <c r="Y108" t="s">
+    <row r="109">
+      <c r="Z109" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="109">
-      <c r="Y109" t="s">
+    <row r="110">
+      <c r="Z110" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="110">
-      <c r="Y110" t="s">
+    <row r="111">
+      <c r="Z111" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="111">
-      <c r="Y111" t="s">
+    <row r="112">
+      <c r="Z112" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="112">
-      <c r="Y112" t="s">
+    <row r="113">
+      <c r="Z113" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="113">
-      <c r="Y113" t="s">
+    <row r="114">
+      <c r="Z114" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="114">
-      <c r="Y114" t="s">
+    <row r="115">
+      <c r="Z115" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="115">
-      <c r="Y115" t="s">
+    <row r="116">
+      <c r="Z116" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="116">
-      <c r="Y116" t="s">
+    <row r="117">
+      <c r="Z117" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="117">
-      <c r="Y117" t="s">
+    <row r="118">
+      <c r="Z118" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="118">
-      <c r="Y118" t="s">
+    <row r="119">
+      <c r="Z119" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="119">
-      <c r="Y119" t="s">
+    <row r="120">
+      <c r="Z120" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="120">
-      <c r="Y120" t="s">
+    <row r="121">
+      <c r="Z121" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="121">
-      <c r="Y121" t="s">
+    <row r="122">
+      <c r="Z122" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="122">
-      <c r="Y122" t="s">
+    <row r="123">
+      <c r="Z123" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="123">
-      <c r="Y123" t="s">
+    <row r="124">
+      <c r="Z124" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="124">
-      <c r="Y124" t="s">
+    <row r="125">
+      <c r="Z125" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="125">
-      <c r="Y125" t="s">
+    <row r="126">
+      <c r="Z126" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="126">
-      <c r="Y126" t="s">
+    <row r="127">
+      <c r="Z127" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="127">
-      <c r="Y127" t="s">
+    <row r="128">
+      <c r="Z128" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="128">
-      <c r="Y128" t="s">
+    <row r="129">
+      <c r="Z129" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="129">
-      <c r="Y129" t="s">
+    <row r="130">
+      <c r="Z130" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="130">
-      <c r="Y130" t="s">
+    <row r="131">
+      <c r="Z131" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="131">
-      <c r="Y131" t="s">
+    <row r="132">
+      <c r="Z132" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="132">
-      <c r="Y132" t="s">
+    <row r="133">
+      <c r="Z133" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="133">
-      <c r="Y133" t="s">
+    <row r="134">
+      <c r="Z134" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="134">
-      <c r="Y134" t="s">
+    <row r="135">
+      <c r="Z135" t="s">
         <v>170</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[rdbms] - [`saveResults(db,sqls,outputDir)`]: code fix to ensure all output are listed in execution output (Excel) and uploaded to the cloud when `nexial.outputToCloud` is set to `true`. - [`saveResult(db,sqls,outputDir)`]: code fix to ensure all output are listed in execution output (Excel) and uploaded to the cloud when `nexial.outputToCloud` is set to `true`.
[web]
- code fix to ensure browser metrics report is uploaded to cloud when `nexial.outputToCloud` to set to `true`.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/script/rdbms-01.xlsx
+++ b/artifact/script/rdbms-01.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17583" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18713" uniqueCount="575">
   <si>
     <t>description</t>
   </si>
@@ -1811,7 +1811,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="544" x14ac:knownFonts="1">
+  <fonts count="576" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5245,8 +5245,210 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="943">
+  <fills count="997">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -10586,8 +10788,314 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="979">
+  <borders count="1043">
     <border>
       <left/>
       <right/>
@@ -18343,6 +18851,658 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -20484,7 +21644,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="569">
+  <cellXfs count="601">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -22161,52 +23321,148 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="915" fontId="527" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="528" fillId="918" borderId="954" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="954" fillId="918" fontId="528" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="529" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="529" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="530" fillId="921" borderId="958" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="958" fillId="921" fontId="530" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="531" fillId="924" borderId="962" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="962" fillId="924" fontId="531" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="532" fillId="927" borderId="966" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="966" fillId="927" fontId="532" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="533" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="533" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="534" fillId="930" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="930" fontId="534" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="535" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="535" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="536" fillId="933" borderId="970" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="970" fillId="933" fontId="536" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="537" fillId="924" borderId="974" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="974" fillId="924" fontId="537" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="538" fillId="936" borderId="978" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="978" fillId="936" fontId="538" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="539" fillId="936" borderId="978" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="978" fillId="936" fontId="539" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="540" fillId="927" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="927" fontId="540" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="541" fillId="939" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="939" fontId="541" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="542" fillId="927" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="927" fontId="542" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="543" fillId="942" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="942" fontId="543" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="986" fillId="945" fontId="544" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="545" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="990" fillId="948" fontId="546" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="994" fillId="951" fontId="547" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="998" fillId="954" fontId="548" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="549" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="957" fontId="550" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="551" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1002" fillId="960" fontId="552" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1006" fillId="951" fontId="553" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1010" fillId="963" fontId="554" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1010" fillId="963" fontId="555" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="954" fontId="556" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="966" fontId="557" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="954" fontId="558" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="969" fontId="559" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="560" fillId="972" borderId="1018" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="561" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="562" fillId="975" borderId="1022" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="563" fillId="978" borderId="1026" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="564" fillId="981" borderId="1030" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="565" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="566" fillId="984" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="567" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="568" fillId="987" borderId="1034" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="569" fillId="978" borderId="1038" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="570" fillId="990" borderId="1042" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="571" fillId="990" borderId="1042" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="572" fillId="981" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="573" fillId="993" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="574" fillId="981" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="575" fillId="996" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>